<commit_message>
spatie installed, UserSeeder, RolePermissionSeeder added, penerapan view khusus role admin
</commit_message>
<xml_diff>
--- a/public/DataArsip/tes import.xlsx
+++ b/public/DataArsip/tes import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Users\bar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C470060E-998E-44E9-B9DA-A0316971633E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFADE880-51A9-4E63-A82F-8B5B13FBA282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{28263804-90BA-4893-B177-E7B169EDA1F6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
   <si>
     <t>KODE PELAKSANA</t>
   </si>
@@ -593,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E5C6E8-55AC-48CF-9A84-8276AD1D358F}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +722,7 @@
     </row>
     <row r="3" spans="1:19" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>22</v>
@@ -888,6 +888,177 @@
         <v>20</v>
       </c>
       <c r="S5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2005</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2005</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2005</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>